<commit_message>
Fix 6 bugs/inefficiencies: pipeline error handling, deploy_nasr glob, KML dedup, image caching
</commit_message>
<xml_diff>
--- a/GUI Files/T38 Planning Aid/wb_list.xlsx
+++ b/GUI Files/T38 Planning Aid/wb_list.xlsx
@@ -959,12 +959,12 @@
       </c>
       <c r="R3" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
+          <t>ADO</t>
         </is>
       </c>
       <c r="S3" s="19" t="inlineStr">
         <is>
-          <t>JMO</t>
+          <t>AWP</t>
         </is>
       </c>
       <c r="T3" s="19" t="n"/>
@@ -1022,17 +1022,17 @@
       </c>
       <c r="Q4" s="19" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="R4" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>BRS</t>
         </is>
       </c>
       <c r="S4" s="19" t="inlineStr">
         <is>
-          <t>WWH</t>
+          <t>JWA</t>
         </is>
       </c>
       <c r="T4" s="19" t="n"/>
@@ -1090,17 +1090,17 @@
       </c>
       <c r="Q5" s="19" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="R5" s="19" t="inlineStr">
         <is>
-          <t>BAP</t>
+          <t>LDE</t>
         </is>
       </c>
       <c r="S5" s="19" t="inlineStr">
         <is>
-          <t>RTH</t>
+          <t>WWH</t>
         </is>
       </c>
       <c r="T5" s="19" t="n"/>
@@ -1163,12 +1163,12 @@
       </c>
       <c r="R6" s="19" t="inlineStr">
         <is>
-          <t>KCO</t>
+          <t>BAP</t>
         </is>
       </c>
       <c r="S6" s="19" t="inlineStr">
         <is>
-          <t>WWH</t>
+          <t>RTH</t>
         </is>
       </c>
       <c r="T6" s="19" t="n"/>
@@ -1227,17 +1227,17 @@
       </c>
       <c r="Q7" s="19" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="R7" s="19" t="inlineStr">
         <is>
-          <t>CJO</t>
+          <t>KCO</t>
         </is>
       </c>
       <c r="S7" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
+          <t>WWH</t>
         </is>
       </c>
       <c r="T7" s="19" t="n"/>
@@ -1301,12 +1301,12 @@
       </c>
       <c r="R8" s="19" t="inlineStr">
         <is>
-          <t>CJO</t>
+          <t>AFU</t>
         </is>
       </c>
       <c r="S8" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
+          <t>BAP</t>
         </is>
       </c>
       <c r="T8" s="19" t="n"/>
@@ -1365,12 +1365,12 @@
       </c>
       <c r="R9" s="19" t="inlineStr">
         <is>
-          <t>AFU</t>
+          <t>CJO</t>
         </is>
       </c>
       <c r="S9" s="19" t="inlineStr">
         <is>
-          <t>BAP</t>
+          <t>CMC</t>
         </is>
       </c>
       <c r="T9" s="19" t="n"/>
@@ -1421,17 +1421,17 @@
       </c>
       <c r="Q10" s="19" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="R10" s="19" t="inlineStr">
         <is>
-          <t>HAS</t>
+          <t>AFU</t>
         </is>
       </c>
       <c r="S10" s="19" t="inlineStr">
         <is>
-          <t>WSM</t>
+          <t>BAP</t>
         </is>
       </c>
       <c r="T10" s="19" t="n"/>
@@ -1541,11 +1541,13 @@
       </c>
       <c r="R12" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
-        </is>
-      </c>
-      <c r="S12" s="19" t="n">
-        <v/>
+          <t>HAS</t>
+        </is>
+      </c>
+      <c r="S12" s="19" t="inlineStr">
+        <is>
+          <t>WSM</t>
+        </is>
       </c>
       <c r="T12" s="19" t="n"/>
       <c r="U12" s="19" t="n"/>
@@ -1601,13 +1603,11 @@
       </c>
       <c r="R13" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
-        </is>
-      </c>
-      <c r="S13" s="19" t="inlineStr">
-        <is>
-          <t>RBL</t>
-        </is>
+          <t>BRS</t>
+        </is>
+      </c>
+      <c r="S13" s="19" t="n">
+        <v/>
       </c>
       <c r="T13" s="19" t="n"/>
       <c r="U13" s="19" t="n"/>
@@ -1706,17 +1706,17 @@
       </c>
       <c r="Q15" s="19" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="R15" s="19" t="inlineStr">
         <is>
-          <t>CBI</t>
+          <t>DDC</t>
         </is>
       </c>
       <c r="S15" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>RBL</t>
         </is>
       </c>
       <c r="T15" s="19" t="n"/>
@@ -1759,16 +1759,18 @@
       </c>
       <c r="Q16" s="19" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="R16" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
-        </is>
-      </c>
-      <c r="S16" s="19" t="n">
-        <v/>
+          <t>CBI</t>
+        </is>
+      </c>
+      <c r="S16" s="19" t="inlineStr">
+        <is>
+          <t>LDE</t>
+        </is>
       </c>
       <c r="T16" s="19" t="n"/>
       <c r="U16" s="19" t="n"/>
@@ -1811,12 +1813,12 @@
       </c>
       <c r="Q17" s="19" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="R17" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
+          <t>SMB</t>
         </is>
       </c>
       <c r="S17" s="19" t="n">
@@ -1867,18 +1869,16 @@
       </c>
       <c r="Q18" s="19" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="R18" s="19" t="inlineStr">
         <is>
-          <t>JPJ</t>
-        </is>
-      </c>
-      <c r="S18" s="19" t="inlineStr">
-        <is>
-          <t>WLS</t>
-        </is>
+          <t>AWP</t>
+        </is>
+      </c>
+      <c r="S18" s="19" t="n">
+        <v/>
       </c>
       <c r="T18" s="19" t="n"/>
       <c r="U18" s="19" t="n"/>
@@ -1920,17 +1920,17 @@
       </c>
       <c r="Q19" s="19" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="R19" s="19" t="inlineStr">
         <is>
-          <t>ADO</t>
+          <t>JPJ</t>
         </is>
       </c>
       <c r="S19" s="19" t="inlineStr">
         <is>
-          <t>HAS</t>
+          <t>WLS</t>
         </is>
       </c>
       <c r="T19" s="19" t="n"/>
@@ -1973,17 +1973,17 @@
       </c>
       <c r="Q20" s="19" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="R20" s="19" t="inlineStr">
         <is>
-          <t>ADO</t>
+          <t>HMK</t>
         </is>
       </c>
       <c r="S20" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>WSM</t>
         </is>
       </c>
       <c r="T20" s="19" t="n"/>
@@ -2027,17 +2027,17 @@
       </c>
       <c r="Q21" s="19" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="R21" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>ADO</t>
         </is>
       </c>
       <c r="S21" s="19" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="T21" s="19" t="n"/>
@@ -3278,12 +3278,12 @@
       </c>
       <c r="R48" s="19" t="inlineStr">
         <is>
-          <t>MBE</t>
+          <t>BRS</t>
         </is>
       </c>
       <c r="S48" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>TIN</t>
         </is>
       </c>
       <c r="T48" s="19" t="n"/>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="R68" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="S68" s="19" t="n">
@@ -4138,7 +4138,7 @@
       </c>
       <c r="R69" s="19" t="inlineStr">
         <is>
-          <t>MAN</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="S69" s="19" t="n">
@@ -4746,13 +4746,11 @@
       </c>
       <c r="R84" s="19" t="inlineStr">
         <is>
-          <t>ASM</t>
-        </is>
-      </c>
-      <c r="S84" s="19" t="inlineStr">
-        <is>
-          <t>CMC</t>
-        </is>
+          <t>AWP</t>
+        </is>
+      </c>
+      <c r="S84" s="19" t="n">
+        <v/>
       </c>
       <c r="T84" s="19" t="n"/>
       <c r="U84" s="19" t="n"/>
@@ -4788,11 +4786,13 @@
       </c>
       <c r="R85" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
-        </is>
-      </c>
-      <c r="S85" s="19" t="n">
-        <v/>
+          <t>ASM</t>
+        </is>
+      </c>
+      <c r="S85" s="19" t="inlineStr">
+        <is>
+          <t>CMC</t>
+        </is>
       </c>
       <c r="T85" s="19" t="n"/>
       <c r="U85" s="19" t="n"/>

</xml_diff>

<commit_message>
Add full KML content to folium map popups (declared distances, NOTE, FOOTER, crew info)
</commit_message>
<xml_diff>
--- a/GUI Files/T38 Planning Aid/wb_list.xlsx
+++ b/GUI Files/T38 Planning Aid/wb_list.xlsx
@@ -872,12 +872,12 @@
       </c>
       <c r="R2" s="19" t="inlineStr">
         <is>
-          <t>LOV</t>
+          <t>BRS</t>
         </is>
       </c>
       <c r="S2" s="19" t="inlineStr">
         <is>
-          <t>PRT</t>
+          <t>JWA</t>
         </is>
       </c>
       <c r="T2" s="19" t="n"/>
@@ -959,12 +959,12 @@
       </c>
       <c r="R3" s="19" t="inlineStr">
         <is>
-          <t>ADO</t>
+          <t>CMC</t>
         </is>
       </c>
       <c r="S3" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
+          <t>JMO</t>
         </is>
       </c>
       <c r="T3" s="19" t="n"/>
@@ -1027,12 +1027,12 @@
       </c>
       <c r="R4" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>JBB</t>
         </is>
       </c>
       <c r="S4" s="19" t="inlineStr">
         <is>
-          <t>JWA</t>
+          <t>JPJ</t>
         </is>
       </c>
       <c r="T4" s="19" t="n"/>
@@ -1090,17 +1090,17 @@
       </c>
       <c r="Q5" s="19" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="R5" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>BRS</t>
         </is>
       </c>
       <c r="S5" s="19" t="inlineStr">
         <is>
-          <t>WWH</t>
+          <t>JWA</t>
         </is>
       </c>
       <c r="T5" s="19" t="n"/>
@@ -1158,17 +1158,17 @@
       </c>
       <c r="Q6" s="19" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="R6" s="19" t="inlineStr">
         <is>
-          <t>BAP</t>
+          <t>LDE</t>
         </is>
       </c>
       <c r="S6" s="19" t="inlineStr">
         <is>
-          <t>RTH</t>
+          <t>WWH</t>
         </is>
       </c>
       <c r="T6" s="19" t="n"/>
@@ -1232,12 +1232,12 @@
       </c>
       <c r="R7" s="19" t="inlineStr">
         <is>
-          <t>KCO</t>
+          <t>CMC</t>
         </is>
       </c>
       <c r="S7" s="19" t="inlineStr">
         <is>
-          <t>WWH</t>
+          <t>PRT</t>
         </is>
       </c>
       <c r="T7" s="19" t="n"/>
@@ -1296,17 +1296,17 @@
       </c>
       <c r="Q8" s="19" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="R8" s="19" t="inlineStr">
         <is>
-          <t>AFU</t>
+          <t>KCO</t>
         </is>
       </c>
       <c r="S8" s="19" t="inlineStr">
         <is>
-          <t>BAP</t>
+          <t>WWH</t>
         </is>
       </c>
       <c r="T8" s="19" t="n"/>
@@ -1365,12 +1365,12 @@
       </c>
       <c r="R9" s="19" t="inlineStr">
         <is>
-          <t>CJO</t>
+          <t>AFU</t>
         </is>
       </c>
       <c r="S9" s="19" t="inlineStr">
         <is>
-          <t>CMC</t>
+          <t>BAP</t>
         </is>
       </c>
       <c r="T9" s="19" t="n"/>
@@ -1426,12 +1426,12 @@
       </c>
       <c r="R10" s="19" t="inlineStr">
         <is>
-          <t>AFU</t>
+          <t>CJO</t>
         </is>
       </c>
       <c r="S10" s="19" t="inlineStr">
         <is>
-          <t>BAP</t>
+          <t>CMC</t>
         </is>
       </c>
       <c r="T10" s="19" t="n"/>
@@ -1478,17 +1478,17 @@
       </c>
       <c r="Q11" s="19" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="R11" s="19" t="inlineStr">
         <is>
-          <t>HAS</t>
+          <t>AFU</t>
         </is>
       </c>
       <c r="S11" s="19" t="inlineStr">
         <is>
-          <t>WSM</t>
+          <t>BAP</t>
         </is>
       </c>
       <c r="T11" s="19" t="n"/>
@@ -1603,11 +1603,13 @@
       </c>
       <c r="R13" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
-        </is>
-      </c>
-      <c r="S13" s="19" t="n">
-        <v/>
+          <t>HAS</t>
+        </is>
+      </c>
+      <c r="S13" s="19" t="inlineStr">
+        <is>
+          <t>WSM</t>
+        </is>
       </c>
       <c r="T13" s="19" t="n"/>
       <c r="U13" s="19" t="n"/>
@@ -1658,13 +1660,11 @@
       </c>
       <c r="R14" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
-        </is>
-      </c>
-      <c r="S14" s="19" t="inlineStr">
-        <is>
-          <t>RBL</t>
-        </is>
+          <t>BRS</t>
+        </is>
+      </c>
+      <c r="S14" s="19" t="n">
+        <v/>
       </c>
       <c r="T14" s="19" t="n"/>
       <c r="U14" s="19" t="n"/>
@@ -1759,17 +1759,17 @@
       </c>
       <c r="Q16" s="19" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="R16" s="19" t="inlineStr">
         <is>
-          <t>CBI</t>
+          <t>DDC</t>
         </is>
       </c>
       <c r="S16" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>RBL</t>
         </is>
       </c>
       <c r="T16" s="19" t="n"/>
@@ -1813,16 +1813,18 @@
       </c>
       <c r="Q17" s="19" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="R17" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
-        </is>
-      </c>
-      <c r="S17" s="19" t="n">
-        <v/>
+          <t>CBI</t>
+        </is>
+      </c>
+      <c r="S17" s="19" t="inlineStr">
+        <is>
+          <t>LDE</t>
+        </is>
       </c>
       <c r="T17" s="19" t="n"/>
       <c r="U17" s="19" t="n"/>
@@ -1869,12 +1871,12 @@
       </c>
       <c r="Q18" s="19" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="R18" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
+          <t>SMB</t>
         </is>
       </c>
       <c r="S18" s="19" t="n">
@@ -1920,17 +1922,17 @@
       </c>
       <c r="Q19" s="19" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="R19" s="19" t="inlineStr">
         <is>
-          <t>JPJ</t>
+          <t>AWP</t>
         </is>
       </c>
       <c r="S19" s="19" t="inlineStr">
         <is>
-          <t>WLS</t>
+          <t>JWG</t>
         </is>
       </c>
       <c r="T19" s="19" t="n"/>
@@ -1973,17 +1975,17 @@
       </c>
       <c r="Q20" s="19" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="R20" s="19" t="inlineStr">
         <is>
-          <t>HMK</t>
+          <t>JPJ</t>
         </is>
       </c>
       <c r="S20" s="19" t="inlineStr">
         <is>
-          <t>WSM</t>
+          <t>WLS</t>
         </is>
       </c>
       <c r="T20" s="19" t="n"/>
@@ -2027,7 +2029,7 @@
       </c>
       <c r="Q21" s="19" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="R21" s="19" t="inlineStr">
@@ -2037,7 +2039,7 @@
       </c>
       <c r="S21" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>HAS</t>
         </is>
       </c>
       <c r="T21" s="19" t="n"/>
@@ -2085,17 +2087,17 @@
       </c>
       <c r="Q22" s="19" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="R22" s="19" t="inlineStr">
         <is>
-          <t>JWA</t>
+          <t>ADO</t>
         </is>
       </c>
       <c r="S22" s="19" t="inlineStr">
         <is>
-          <t>MAN</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="T22" s="19" t="n"/>
@@ -2138,17 +2140,17 @@
       </c>
       <c r="Q23" s="19" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="R23" s="19" t="inlineStr">
         <is>
-          <t>CBI</t>
+          <t>JWA</t>
         </is>
       </c>
       <c r="S23" s="19" t="inlineStr">
         <is>
-          <t>LDE</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="T23" s="19" t="n"/>
@@ -2250,12 +2252,12 @@
       </c>
       <c r="Q25" s="19" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="R25" s="19" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>CBI</t>
         </is>
       </c>
       <c r="S25" s="19" t="inlineStr">
@@ -2303,17 +2305,17 @@
       </c>
       <c r="Q26" s="19" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="R26" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="S26" s="19" t="inlineStr">
         <is>
-          <t>HMK</t>
+          <t>LDE</t>
         </is>
       </c>
       <c r="T26" s="19" t="n"/>
@@ -2357,17 +2359,17 @@
       </c>
       <c r="Q27" s="19" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="R27" s="19" t="inlineStr">
         <is>
-          <t>JMO</t>
+          <t>GLO</t>
         </is>
       </c>
       <c r="S27" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>HMK</t>
         </is>
       </c>
       <c r="T27" s="19" t="n"/>
@@ -2411,17 +2413,17 @@
       </c>
       <c r="Q28" s="19" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="R28" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>JMO</t>
         </is>
       </c>
       <c r="S28" s="19" t="inlineStr">
         <is>
-          <t>LOV</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="T28" s="19" t="n"/>
@@ -2465,17 +2467,17 @@
       </c>
       <c r="Q29" s="19" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="R29" s="19" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>BRS</t>
         </is>
       </c>
       <c r="S29" s="19" t="inlineStr">
         <is>
-          <t>TIN</t>
+          <t>LOV</t>
         </is>
       </c>
       <c r="T29" s="19" t="n"/>
@@ -2524,12 +2526,12 @@
       </c>
       <c r="R30" s="19" t="inlineStr">
         <is>
-          <t>CBI</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="S30" s="19" t="inlineStr">
         <is>
-          <t>SMB</t>
+          <t>TIN</t>
         </is>
       </c>
       <c r="T30" s="19" t="n"/>
@@ -2573,16 +2575,18 @@
       </c>
       <c r="Q31" s="19" t="inlineStr">
         <is>
-          <t>2025-11-19</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="R31" s="19" t="inlineStr">
         <is>
-          <t>MAN</t>
-        </is>
-      </c>
-      <c r="S31" s="19" t="n">
-        <v/>
+          <t>CBI</t>
+        </is>
+      </c>
+      <c r="S31" s="19" t="inlineStr">
+        <is>
+          <t>SMB</t>
+        </is>
       </c>
       <c r="T31" s="19" t="n"/>
       <c r="U31" s="19" t="n"/>
@@ -2618,13 +2622,11 @@
       </c>
       <c r="R32" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
-        </is>
-      </c>
-      <c r="S32" s="19" t="inlineStr">
-        <is>
-          <t>FRU</t>
-        </is>
+          <t>MAN</t>
+        </is>
+      </c>
+      <c r="S32" s="19" t="n">
+        <v/>
       </c>
       <c r="T32" s="19" t="n"/>
       <c r="U32" s="19" t="n"/>
@@ -2655,17 +2657,17 @@
       </c>
       <c r="Q33" s="19" t="inlineStr">
         <is>
-          <t>2025-11-14</t>
+          <t>2025-11-19</t>
         </is>
       </c>
       <c r="R33" s="19" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>BRS</t>
         </is>
       </c>
       <c r="S33" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>FRU</t>
         </is>
       </c>
       <c r="T33" s="19" t="n"/>
@@ -2697,16 +2699,18 @@
       </c>
       <c r="Q34" s="19" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-14</t>
         </is>
       </c>
       <c r="R34" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
-        </is>
-      </c>
-      <c r="S34" s="19" t="n">
-        <v/>
+          <t>LAO</t>
+        </is>
+      </c>
+      <c r="S34" s="19" t="inlineStr">
+        <is>
+          <t>RJC</t>
+        </is>
       </c>
       <c r="T34" s="19" t="n"/>
       <c r="U34" s="19" t="n"/>
@@ -2737,18 +2741,16 @@
       </c>
       <c r="Q35" s="19" t="inlineStr">
         <is>
-          <t>2025-11-05</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="R35" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
-        </is>
-      </c>
-      <c r="S35" s="19" t="inlineStr">
-        <is>
-          <t>BNE</t>
-        </is>
+          <t>GLO</t>
+        </is>
+      </c>
+      <c r="S35" s="19" t="n">
+        <v/>
       </c>
       <c r="T35" s="19" t="n"/>
       <c r="U35" s="19" t="n"/>
@@ -2779,17 +2781,17 @@
       </c>
       <c r="Q36" s="19" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-11-05</t>
         </is>
       </c>
       <c r="R36" s="19" t="inlineStr">
         <is>
-          <t>DAR</t>
+          <t>AWP</t>
         </is>
       </c>
       <c r="S36" s="19" t="inlineStr">
         <is>
-          <t>RTH</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="T36" s="19" t="n"/>
@@ -2821,16 +2823,18 @@
       </c>
       <c r="Q37" s="19" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="R37" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
-        </is>
-      </c>
-      <c r="S37" s="19" t="n">
-        <v/>
+          <t>DAR</t>
+        </is>
+      </c>
+      <c r="S37" s="19" t="inlineStr">
+        <is>
+          <t>RTH</t>
+        </is>
       </c>
       <c r="T37" s="19" t="n"/>
       <c r="U37" s="19" t="n"/>
@@ -2941,12 +2945,12 @@
       </c>
       <c r="Q40" s="19" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="R40" s="19" t="inlineStr">
         <is>
-          <t>GLO</t>
+          <t>DDC</t>
         </is>
       </c>
       <c r="S40" s="19" t="n">
@@ -2981,18 +2985,16 @@
       </c>
       <c r="Q41" s="19" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="R41" s="19" t="inlineStr">
         <is>
-          <t>BAP</t>
-        </is>
-      </c>
-      <c r="S41" s="19" t="inlineStr">
-        <is>
-          <t>FRU</t>
-        </is>
+          <t>GLO</t>
+        </is>
+      </c>
+      <c r="S41" s="19" t="n">
+        <v/>
       </c>
       <c r="T41" s="19" t="n"/>
       <c r="U41" s="19" t="n"/>
@@ -3023,17 +3025,17 @@
       </c>
       <c r="Q42" s="19" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="R42" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>BAP</t>
         </is>
       </c>
       <c r="S42" s="19" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>FRU</t>
         </is>
       </c>
       <c r="T42" s="19" t="n"/>
@@ -3278,12 +3280,12 @@
       </c>
       <c r="R48" s="19" t="inlineStr">
         <is>
-          <t>BRS</t>
+          <t>MBE</t>
         </is>
       </c>
       <c r="S48" s="19" t="inlineStr">
         <is>
-          <t>TIN</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="T48" s="19" t="n"/>
@@ -4018,11 +4020,13 @@
       </c>
       <c r="R66" s="19" t="inlineStr">
         <is>
+          <t>JWG</t>
+        </is>
+      </c>
+      <c r="S66" s="19" t="inlineStr">
+        <is>
           <t>SMB</t>
         </is>
-      </c>
-      <c r="S66" s="19" t="n">
-        <v/>
       </c>
       <c r="T66" s="19" t="n"/>
       <c r="U66" s="19" t="n"/>
@@ -4098,7 +4102,7 @@
       </c>
       <c r="R68" s="19" t="inlineStr">
         <is>
-          <t>MAN</t>
+          <t>RJC</t>
         </is>
       </c>
       <c r="S68" s="19" t="n">
@@ -4138,7 +4142,7 @@
       </c>
       <c r="R69" s="19" t="inlineStr">
         <is>
-          <t>RJC</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="S69" s="19" t="n">
@@ -4583,8 +4587,10 @@
           <t>GLO</t>
         </is>
       </c>
-      <c r="S80" s="19" t="n">
-        <v/>
+      <c r="S80" s="19" t="inlineStr">
+        <is>
+          <t>WLS</t>
+        </is>
       </c>
       <c r="T80" s="19" t="n"/>
       <c r="U80" s="19" t="n"/>
@@ -4623,10 +4629,8 @@
           <t>GLO</t>
         </is>
       </c>
-      <c r="S81" s="19" t="inlineStr">
-        <is>
-          <t>WLS</t>
-        </is>
+      <c r="S81" s="19" t="n">
+        <v/>
       </c>
       <c r="T81" s="19" t="n"/>
       <c r="U81" s="19" t="n"/>
@@ -4746,11 +4750,13 @@
       </c>
       <c r="R84" s="19" t="inlineStr">
         <is>
-          <t>AWP</t>
-        </is>
-      </c>
-      <c r="S84" s="19" t="n">
-        <v/>
+          <t>ASM</t>
+        </is>
+      </c>
+      <c r="S84" s="19" t="inlineStr">
+        <is>
+          <t>CMC</t>
+        </is>
       </c>
       <c r="T84" s="19" t="n"/>
       <c r="U84" s="19" t="n"/>
@@ -4786,13 +4792,11 @@
       </c>
       <c r="R85" s="19" t="inlineStr">
         <is>
-          <t>ASM</t>
-        </is>
-      </c>
-      <c r="S85" s="19" t="inlineStr">
-        <is>
-          <t>CMC</t>
-        </is>
+          <t>AWP</t>
+        </is>
+      </c>
+      <c r="S85" s="19" t="n">
+        <v/>
       </c>
       <c r="T85" s="19" t="n"/>
       <c r="U85" s="19" t="n"/>
@@ -5604,11 +5608,13 @@
       </c>
       <c r="R105" s="19" t="inlineStr">
         <is>
-          <t>DDC</t>
-        </is>
-      </c>
-      <c r="S105" s="19" t="n">
-        <v/>
+          <t>LOV</t>
+        </is>
+      </c>
+      <c r="S105" s="19" t="inlineStr">
+        <is>
+          <t>RTH</t>
+        </is>
       </c>
       <c r="T105" s="19" t="n"/>
       <c r="U105" s="19" t="n"/>
@@ -5644,13 +5650,11 @@
       </c>
       <c r="R106" s="19" t="inlineStr">
         <is>
-          <t>LOV</t>
-        </is>
-      </c>
-      <c r="S106" s="19" t="inlineStr">
-        <is>
-          <t>RTH</t>
-        </is>
+          <t>DDC</t>
+        </is>
+      </c>
+      <c r="S106" s="19" t="n">
+        <v/>
       </c>
       <c r="T106" s="19" t="n"/>
       <c r="U106" s="19" t="n"/>

</xml_diff>